<commit_message>
Photos of Emp and Cust added to db and spring boot
</commit_message>
<xml_diff>
--- a/Other Files/Work Tracking.xlsx
+++ b/Other Files/Work Tracking.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FinalProject\Other Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7E50B0-D4FC-4206-B377-2DB88E4FC40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983A4C12-101F-4838-BDAB-BAFA2DE31885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{0B1627D4-195F-4C4A-9E74-68524C6C240B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{0B1627D4-195F-4C4A-9E74-68524C6C240B}"/>
   </bookViews>
   <sheets>
     <sheet name="TABLES" sheetId="1" r:id="rId1"/>
     <sheet name="QUERY" sheetId="2" r:id="rId2"/>
     <sheet name="FRONTEND" sheetId="3" r:id="rId3"/>
+    <sheet name="JWT" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="87">
   <si>
     <t>TABLES</t>
   </si>
@@ -266,6 +267,39 @@
   </si>
   <si>
     <t>Salesman</t>
+  </si>
+  <si>
+    <t>pom.xml</t>
+  </si>
+  <si>
+    <t>MumsApplication.java</t>
+  </si>
+  <si>
+    <t>application.properties</t>
+  </si>
+  <si>
+    <t>config package</t>
+  </si>
+  <si>
+    <t>security package</t>
+  </si>
+  <si>
+    <t>LoginRepo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login </t>
+  </si>
+  <si>
+    <t>AppConstants</t>
+  </si>
+  <si>
+    <t>SalesmanServiceImpl</t>
+  </si>
+  <si>
+    <t>AuthController</t>
+  </si>
+  <si>
+    <t>JwtAuthResponse- payload</t>
   </si>
 </sst>
 </file>
@@ -987,7 +1021,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE44FD0-900A-49F6-A45C-930FE5ABD856}">
   <dimension ref="A2:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
@@ -1122,4 +1156,77 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{144035DF-CD97-48CC-8F5C-1B861B4A3B53}">
+  <dimension ref="A2:A16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Almost final Backend update with JWT
</commit_message>
<xml_diff>
--- a/Other Files/Work Tracking.xlsx
+++ b/Other Files/Work Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FinalProject\Other Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983A4C12-101F-4838-BDAB-BAFA2DE31885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF167ED-28B9-4970-9DA3-7CAB1512B414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{0B1627D4-195F-4C4A-9E74-68524C6C240B}"/>
   </bookViews>
@@ -306,7 +306,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,6 +357,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -378,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -386,6 +393,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -703,7 +711,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -804,7 +812,7 @@
       <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="7" t="s">
         <v>24</v>
       </c>
     </row>
@@ -818,7 +826,7 @@
       <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="7" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>